<commit_message>
Major updates to spreadsheets. Began to create visualizations via Tableau.
</commit_message>
<xml_diff>
--- a/spreadsheets/US_Sub4_Milers.xlsx
+++ b/spreadsheets/US_Sub4_Milers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ljcoo\NSS\Projects\United_States_Sub_4_Milers_Database\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61F954A2-FA2E-4D76-A28B-1A0CE6BEDF58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AECAE3D-6C43-4B00-B9E9-ECEDA712E9BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" firstSheet="5" activeTab="7" xr2:uid="{FC2F9DD0-DB5D-4A46-B58C-40A2751618EA}"/>
+    <workbookView xWindow="3432" yWindow="1416" windowWidth="17280" windowHeight="10044" firstSheet="2" activeTab="4" xr2:uid="{FC2F9DD0-DB5D-4A46-B58C-40A2751618EA}"/>
   </bookViews>
   <sheets>
     <sheet name="US Sub-4 Milers" sheetId="1" r:id="rId1"/>
@@ -38924,10 +38924,13 @@
   <dimension ref="A1:E64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="D65" sqref="D65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="8.88671875" style="22"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
@@ -38939,7 +38942,7 @@
       <c r="C1" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="21" t="s">
         <v>1736</v>
       </c>
       <c r="E1" s="5" t="s">
@@ -38958,7 +38961,9 @@
         <f>AVERAGE('US Sub-4 Milers'!G2)</f>
         <v>2.7627314814814819E-3</v>
       </c>
-      <c r="D2" s="2"/>
+      <c r="D2" s="22">
+        <v>238.7</v>
+      </c>
       <c r="E2" t="s">
         <v>26</v>
       </c>
@@ -38975,7 +38980,9 @@
         <f>AVERAGE('US Sub-4 Milers'!G3:G4)</f>
         <v>2.7581018518518519E-3</v>
       </c>
-      <c r="D3" s="2"/>
+      <c r="D3" s="22">
+        <v>238.3</v>
+      </c>
       <c r="E3" t="s">
         <v>27</v>
       </c>
@@ -38992,7 +38999,9 @@
         <f>AVERAGE('US Sub-4 Milers'!G5:G9)</f>
         <v>2.7652083333333331E-3</v>
       </c>
-      <c r="D4" s="2"/>
+      <c r="D4" s="22">
+        <v>238.9</v>
+      </c>
       <c r="E4" t="s">
         <v>27</v>
       </c>
@@ -39009,7 +39018,9 @@
         <f>AVERAGE('US Sub-4 Milers'!G10)</f>
         <v>2.7685185185185187E-3</v>
       </c>
-      <c r="D5" s="2"/>
+      <c r="D5" s="22">
+        <v>239.2</v>
+      </c>
       <c r="E5" t="s">
         <v>27</v>
       </c>
@@ -39026,7 +39037,9 @@
         <f>AVERAGE('US Sub-4 Milers'!G11:G15)</f>
         <v>2.7604166666666667E-3</v>
       </c>
-      <c r="D6" s="2"/>
+      <c r="D6" s="22">
+        <v>238.5</v>
+      </c>
       <c r="E6" t="s">
         <v>27</v>
       </c>
@@ -39043,7 +39056,9 @@
         <f>AVERAGE('US Sub-4 Milers'!G16)</f>
         <v>2.7557870370370371E-3</v>
       </c>
-      <c r="D7" s="2"/>
+      <c r="D7" s="22">
+        <v>238.1</v>
+      </c>
       <c r="E7" t="s">
         <v>27</v>
       </c>
@@ -39060,7 +39075,9 @@
         <f>AVERAGE('US Sub-4 Milers'!G17:G21)</f>
         <v>2.7696759259259259E-3</v>
       </c>
-      <c r="D8" s="2"/>
+      <c r="D8" s="22">
+        <v>239.3</v>
+      </c>
       <c r="E8" t="s">
         <v>27</v>
       </c>
@@ -39077,7 +39094,9 @@
         <f>AVERAGE('US Sub-4 Milers'!G22:G26)</f>
         <v>2.756712962962963E-3</v>
       </c>
-      <c r="D9" s="2"/>
+      <c r="D9" s="22">
+        <v>238.2</v>
+      </c>
       <c r="E9" t="s">
         <v>27</v>
       </c>
@@ -39094,7 +39113,9 @@
         <f>AVERAGE('US Sub-4 Milers'!G27:G30)</f>
         <v>2.7618634259259259E-3</v>
       </c>
-      <c r="D10" s="2"/>
+      <c r="D10" s="22">
+        <v>238.6</v>
+      </c>
       <c r="E10" t="s">
         <v>27</v>
       </c>
@@ -39111,7 +39132,9 @@
         <f>AVERAGE('US Sub-4 Milers'!G31:G32)</f>
         <v>2.7656250000000003E-3</v>
       </c>
-      <c r="D11" s="2"/>
+      <c r="D11" s="22">
+        <v>239</v>
+      </c>
       <c r="E11" t="s">
         <v>27</v>
       </c>
@@ -39128,7 +39151,9 @@
         <f>AVERAGE('US Sub-4 Milers'!G33:G40)</f>
         <v>2.7653356481481483E-3</v>
       </c>
-      <c r="D12" s="2"/>
+      <c r="D12" s="22">
+        <v>238.9</v>
+      </c>
       <c r="E12" t="s">
         <v>115</v>
       </c>
@@ -39145,7 +39170,9 @@
         <f>AVERAGE('US Sub-4 Milers'!G41:G47)</f>
         <v>2.7713293650793651E-3</v>
       </c>
-      <c r="D13" s="2"/>
+      <c r="D13" s="22">
+        <v>239.4</v>
+      </c>
       <c r="E13" t="s">
         <v>115</v>
       </c>
@@ -39162,7 +39189,9 @@
         <f>AVERAGE('US Sub-4 Milers'!G48:G51)</f>
         <v>2.7690972222222223E-3</v>
       </c>
-      <c r="D14" s="2"/>
+      <c r="D14" s="22">
+        <v>239.2</v>
+      </c>
       <c r="E14" t="s">
         <v>115</v>
       </c>
@@ -39179,7 +39208,9 @@
         <f>AVERAGE('US Sub-4 Milers'!G52:G63)</f>
         <v>2.7635995370370371E-3</v>
       </c>
-      <c r="D15" s="2"/>
+      <c r="D15" s="22">
+        <v>238.8</v>
+      </c>
       <c r="E15" t="s">
         <v>115</v>
       </c>
@@ -39196,7 +39227,9 @@
         <f>AVERAGE('US Sub-4 Milers'!G64:G74)</f>
         <v>2.759890572390573E-3</v>
       </c>
-      <c r="D16" s="2"/>
+      <c r="D16" s="22">
+        <v>238.5</v>
+      </c>
       <c r="E16" t="s">
         <v>115</v>
       </c>
@@ -39213,7 +39246,9 @@
         <f>AVERAGE('US Sub-4 Milers'!G75:G81)</f>
         <v>2.7619047619047614E-3</v>
       </c>
-      <c r="D17" s="2"/>
+      <c r="D17" s="22">
+        <v>238.6</v>
+      </c>
       <c r="E17" t="s">
         <v>115</v>
       </c>
@@ -39230,7 +39265,9 @@
         <f>AVERAGE('US Sub-4 Milers'!G82:G83)</f>
         <v>2.7702546296296295E-3</v>
       </c>
-      <c r="D18" s="2"/>
+      <c r="D18" s="22">
+        <v>239.3</v>
+      </c>
       <c r="E18" t="s">
         <v>115</v>
       </c>
@@ -39247,7 +39284,9 @@
         <f>AVERAGE('US Sub-4 Milers'!G84:G87)</f>
         <v>2.7648726851851849E-3</v>
       </c>
-      <c r="D19" s="2"/>
+      <c r="D19" s="22">
+        <v>238.9</v>
+      </c>
       <c r="E19" t="s">
         <v>115</v>
       </c>
@@ -39264,7 +39303,9 @@
         <f>AVERAGE('US Sub-4 Milers'!G88:G96)</f>
         <v>2.7649948559670778E-3</v>
       </c>
-      <c r="D20" s="2"/>
+      <c r="D20" s="22">
+        <v>238.9</v>
+      </c>
       <c r="E20" t="s">
         <v>115</v>
       </c>
@@ -39281,7 +39322,9 @@
         <f>AVERAGE('US Sub-4 Milers'!G97:G100)</f>
         <v>2.7609664351851853E-3</v>
       </c>
-      <c r="D21" s="2"/>
+      <c r="D21" s="22">
+        <v>238.5</v>
+      </c>
       <c r="E21" t="s">
         <v>115</v>
       </c>
@@ -39298,7 +39341,9 @@
         <f>AVERAGE('US Sub-4 Milers'!G101:G108)</f>
         <v>2.7611111111111109E-3</v>
       </c>
-      <c r="D22" s="2"/>
+      <c r="D22" s="22">
+        <v>238.6</v>
+      </c>
       <c r="E22" t="s">
         <v>116</v>
       </c>
@@ -39315,7 +39360,9 @@
         <f>AVERAGE('US Sub-4 Milers'!G109:G117)</f>
         <v>2.7399305555555558E-3</v>
       </c>
-      <c r="D23" s="2"/>
+      <c r="D23" s="22">
+        <v>236.7</v>
+      </c>
       <c r="E23" t="s">
         <v>116</v>
       </c>
@@ -39332,7 +39379,9 @@
         <f>AVERAGE('US Sub-4 Milers'!G118:G126)</f>
         <v>2.7569444444444447E-3</v>
       </c>
-      <c r="D24" s="2"/>
+      <c r="D24" s="22">
+        <v>238.2</v>
+      </c>
       <c r="E24" t="s">
         <v>116</v>
       </c>
@@ -39349,7 +39398,9 @@
         <f>AVERAGE('US Sub-4 Milers'!G127:G134)</f>
         <v>2.7614004629629625E-3</v>
       </c>
-      <c r="D25" s="2"/>
+      <c r="D25" s="22">
+        <v>238.6</v>
+      </c>
       <c r="E25" t="s">
         <v>116</v>
       </c>
@@ -39366,7 +39417,9 @@
         <f>AVERAGE('US Sub-4 Milers'!G135:G138)</f>
         <v>2.7603877314814813E-3</v>
       </c>
-      <c r="D26" s="2"/>
+      <c r="D26" s="22">
+        <v>238.5</v>
+      </c>
       <c r="E26" t="s">
         <v>116</v>
       </c>
@@ -39383,7 +39436,9 @@
         <f>AVERAGE('US Sub-4 Milers'!G139:G143)</f>
         <v>2.7675231481481483E-3</v>
       </c>
-      <c r="D27" s="2"/>
+      <c r="D27" s="22">
+        <v>239.1</v>
+      </c>
       <c r="E27" t="s">
         <v>116</v>
       </c>
@@ -39400,7 +39455,9 @@
         <f>AVERAGE('US Sub-4 Milers'!G144:G149)</f>
         <v>2.7684413580246919E-3</v>
       </c>
-      <c r="D28" s="2"/>
+      <c r="D28" s="22">
+        <v>239.2</v>
+      </c>
       <c r="E28" t="s">
         <v>116</v>
       </c>
@@ -39417,7 +39474,9 @@
         <f>AVERAGE('US Sub-4 Milers'!G150:G154)</f>
         <v>2.7656249999999999E-3</v>
       </c>
-      <c r="D29" s="2"/>
+      <c r="D29" s="22">
+        <v>239</v>
+      </c>
       <c r="E29" t="s">
         <v>116</v>
       </c>
@@ -39434,7 +39493,9 @@
         <f>AVERAGE('US Sub-4 Milers'!G155:G162)</f>
         <v>2.7584924768518518E-3</v>
       </c>
-      <c r="D30" s="2"/>
+      <c r="D30" s="22">
+        <v>238.3</v>
+      </c>
       <c r="E30" t="s">
         <v>116</v>
       </c>
@@ -39451,7 +39512,9 @@
         <f>AVERAGE('US Sub-4 Milers'!G163:G169)</f>
         <v>2.7692294973544981E-3</v>
       </c>
-      <c r="D31" s="2"/>
+      <c r="D31" s="22">
+        <v>239.3</v>
+      </c>
       <c r="E31" t="s">
         <v>116</v>
       </c>
@@ -39468,7 +39531,9 @@
         <f>AVERAGE('US Sub-4 Milers'!G170:G172)</f>
         <v>2.7702160493827161E-3</v>
       </c>
-      <c r="D32" s="2"/>
+      <c r="D32" s="22">
+        <v>239.3</v>
+      </c>
       <c r="E32" t="s">
         <v>117</v>
       </c>
@@ -39485,7 +39550,9 @@
         <f>AVERAGE('US Sub-4 Milers'!G173:G184)</f>
         <v>2.7594714506172843E-3</v>
       </c>
-      <c r="D33" s="2"/>
+      <c r="D33" s="22">
+        <v>238.4</v>
+      </c>
       <c r="E33" t="s">
         <v>117</v>
       </c>
@@ -39502,7 +39569,9 @@
         <f>AVERAGE('US Sub-4 Milers'!G185:G188)</f>
         <v>2.7524305555555553E-3</v>
       </c>
-      <c r="D34" s="2"/>
+      <c r="D34" s="22">
+        <v>237.8</v>
+      </c>
       <c r="E34" t="s">
         <v>117</v>
       </c>
@@ -39519,7 +39588,9 @@
         <f>AVERAGE('US Sub-4 Milers'!G189:G195)</f>
         <v>2.7632275132275135E-3</v>
       </c>
-      <c r="D35" s="2"/>
+      <c r="D35" s="22">
+        <v>238.7</v>
+      </c>
       <c r="E35" t="s">
         <v>117</v>
       </c>
@@ -39536,7 +39607,9 @@
         <f>AVERAGE('US Sub-4 Milers'!G196:G204)</f>
         <v>2.7645961934156375E-3</v>
       </c>
-      <c r="D36" s="2"/>
+      <c r="D36" s="22">
+        <v>238.9</v>
+      </c>
       <c r="E36" t="s">
         <v>117</v>
       </c>
@@ -39553,7 +39626,9 @@
         <f>AVERAGE('US Sub-4 Milers'!G205:G210)</f>
         <v>2.760011574074074E-3</v>
       </c>
-      <c r="D37" s="2"/>
+      <c r="D37" s="22">
+        <v>238.5</v>
+      </c>
       <c r="E37" t="s">
         <v>117</v>
       </c>
@@ -39570,7 +39645,9 @@
         <f>AVERAGE('US Sub-4 Milers'!G211:G212)</f>
         <v>2.7662037037037039E-3</v>
       </c>
-      <c r="D38" s="2"/>
+      <c r="D38" s="22">
+        <v>239</v>
+      </c>
       <c r="E38" t="s">
         <v>117</v>
       </c>
@@ -39587,7 +39664,9 @@
         <f>AVERAGE('US Sub-4 Milers'!G213:G220)</f>
         <v>2.7585214120370368E-3</v>
       </c>
-      <c r="D39" s="2"/>
+      <c r="D39" s="22">
+        <v>238.3</v>
+      </c>
       <c r="E39" t="s">
         <v>117</v>
       </c>
@@ -39604,7 +39683,9 @@
         <f>AVERAGE('US Sub-4 Milers'!G221:G228)</f>
         <v>2.7706163194444445E-3</v>
       </c>
-      <c r="D40" s="2"/>
+      <c r="D40" s="22">
+        <v>239.4</v>
+      </c>
       <c r="E40" t="s">
         <v>117</v>
       </c>
@@ -39621,7 +39702,9 @@
         <f>AVERAGE('US Sub-4 Milers'!G229:G232)</f>
         <v>2.7553530092592595E-3</v>
       </c>
-      <c r="D41" s="2"/>
+      <c r="D41" s="22">
+        <v>238.1</v>
+      </c>
       <c r="E41" t="s">
         <v>117</v>
       </c>
@@ -39638,7 +39721,9 @@
         <f>AVERAGE('US Sub-4 Milers'!G233:G238)</f>
         <v>2.7691358024691357E-3</v>
       </c>
-      <c r="D42" s="2"/>
+      <c r="D42" s="22">
+        <v>239.3</v>
+      </c>
       <c r="E42" t="s">
         <v>118</v>
       </c>
@@ -39655,7 +39740,9 @@
         <f>AVERAGE('US Sub-4 Milers'!G239:G246)</f>
         <v>2.7673321759259257E-3</v>
       </c>
-      <c r="D43" s="2"/>
+      <c r="D43" s="22">
+        <v>239.1</v>
+      </c>
       <c r="E43" t="s">
         <v>118</v>
       </c>
@@ -39672,7 +39759,9 @@
         <f>AVERAGE('US Sub-4 Milers'!G247:G253)</f>
         <v>2.7695601851851848E-3</v>
       </c>
-      <c r="D44" s="2"/>
+      <c r="D44" s="22">
+        <v>239.5</v>
+      </c>
       <c r="E44" t="s">
         <v>118</v>
       </c>
@@ -39689,7 +39778,9 @@
         <f>AVERAGE('US Sub-4 Milers'!G254:G258)</f>
         <v>2.7628703703703708E-3</v>
       </c>
-      <c r="D45" s="2"/>
+      <c r="D45" s="22">
+        <v>238.7</v>
+      </c>
       <c r="E45" t="s">
         <v>118</v>
       </c>
@@ -39706,7 +39797,9 @@
         <f>AVERAGE('US Sub-4 Milers'!G259:G265)</f>
         <v>2.7654927248677249E-3</v>
       </c>
-      <c r="D46" s="2"/>
+      <c r="D46" s="22">
+        <v>238.9</v>
+      </c>
       <c r="E46" t="s">
         <v>118</v>
       </c>
@@ -39723,7 +39816,9 @@
         <f>AVERAGE('US Sub-4 Milers'!G266:G273)</f>
         <v>2.7516637731481476E-3</v>
       </c>
-      <c r="D47" s="2"/>
+      <c r="D47" s="22">
+        <v>237.7</v>
+      </c>
       <c r="E47" t="s">
         <v>118</v>
       </c>
@@ -39740,7 +39835,9 @@
         <f>AVERAGE('US Sub-4 Milers'!G274:G285)</f>
         <v>2.7652006172839507E-3</v>
       </c>
-      <c r="D48" s="2"/>
+      <c r="D48" s="22">
+        <v>238.9</v>
+      </c>
       <c r="E48" t="s">
         <v>118</v>
       </c>
@@ -39757,7 +39854,9 @@
         <f>AVERAGE('US Sub-4 Milers'!G286:G298)</f>
         <v>2.7620281339031339E-3</v>
       </c>
-      <c r="D49" s="2"/>
+      <c r="D49" s="22">
+        <v>238.6</v>
+      </c>
       <c r="E49" t="s">
         <v>118</v>
       </c>
@@ -39774,7 +39873,9 @@
         <f>AVERAGE('US Sub-4 Milers'!G299:G313)</f>
         <v>2.7637422839506174E-3</v>
       </c>
-      <c r="D50" s="2"/>
+      <c r="D50" s="22">
+        <v>238.8</v>
+      </c>
       <c r="E50" t="s">
         <v>118</v>
       </c>
@@ -39791,7 +39892,9 @@
         <f>AVERAGE('US Sub-4 Milers'!G314:G330)</f>
         <v>2.7568218954248367E-3</v>
       </c>
-      <c r="D51" s="2"/>
+      <c r="D51" s="22">
+        <v>238.2</v>
+      </c>
       <c r="E51" t="s">
         <v>118</v>
       </c>
@@ -39808,7 +39911,9 @@
         <f>AVERAGE('US Sub-4 Milers'!G331:G350)</f>
         <v>2.7666087962962965E-3</v>
       </c>
-      <c r="D52" s="2"/>
+      <c r="D52" s="22">
+        <v>239</v>
+      </c>
       <c r="E52" t="s">
         <v>119</v>
       </c>
@@ -39825,7 +39930,9 @@
         <f>AVERAGE('US Sub-4 Milers'!G351:G362)</f>
         <v>2.7589216820987656E-3</v>
       </c>
-      <c r="D53" s="2"/>
+      <c r="D53" s="22">
+        <v>238.4</v>
+      </c>
       <c r="E53" t="s">
         <v>119</v>
       </c>
@@ -39842,7 +39949,9 @@
         <f>AVERAGE('US Sub-4 Milers'!G363:G385)</f>
         <v>2.7658514492753632E-3</v>
       </c>
-      <c r="D54" s="2"/>
+      <c r="D54" s="22">
+        <v>239</v>
+      </c>
       <c r="E54" t="s">
         <v>119</v>
       </c>
@@ -39859,7 +39968,9 @@
         <f>AVERAGE('US Sub-4 Milers'!G386:G408)</f>
         <v>2.7647141706924313E-3</v>
       </c>
-      <c r="D55" s="2"/>
+      <c r="D55" s="22">
+        <v>238.9</v>
+      </c>
       <c r="E55" t="s">
         <v>119</v>
       </c>
@@ -39876,7 +39987,9 @@
         <f>AVERAGE('US Sub-4 Milers'!G409:G426)</f>
         <v>2.7619984567901238E-3</v>
       </c>
-      <c r="D56" s="2"/>
+      <c r="D56" s="22">
+        <v>238.6</v>
+      </c>
       <c r="E56" t="s">
         <v>119</v>
       </c>
@@ -39893,7 +40006,9 @@
         <f>AVERAGE('US Sub-4 Milers'!G427:G450)</f>
         <v>2.7656925154320986E-3</v>
       </c>
-      <c r="D57" s="2"/>
+      <c r="D57" s="22">
+        <v>239</v>
+      </c>
       <c r="E57" t="s">
         <v>119</v>
       </c>
@@ -39910,7 +40025,9 @@
         <f>AVERAGE('US Sub-4 Milers'!G451:G477)</f>
         <v>2.7622899519890256E-3</v>
       </c>
-      <c r="D58" s="2"/>
+      <c r="D58" s="22">
+        <v>238.7</v>
+      </c>
       <c r="E58" t="s">
         <v>119</v>
       </c>
@@ -39927,7 +40044,9 @@
         <f>AVERAGE('US Sub-4 Milers'!G478:G494)</f>
         <v>2.7646241830065355E-3</v>
       </c>
-      <c r="D59" s="2"/>
+      <c r="D59" s="22">
+        <v>238.9</v>
+      </c>
       <c r="E59" t="s">
         <v>119</v>
       </c>
@@ -39944,7 +40063,9 @@
         <f>AVERAGE('US Sub-4 Milers'!G495:G523)</f>
         <v>2.7636454342273306E-3</v>
       </c>
-      <c r="D60" s="2"/>
+      <c r="D60" s="22">
+        <v>238.8</v>
+      </c>
       <c r="E60" t="s">
         <v>119</v>
       </c>
@@ -39961,7 +40082,9 @@
         <f>AVERAGE('US Sub-4 Milers'!G524:G545)</f>
         <v>2.7666561447811447E-3</v>
       </c>
-      <c r="D61" s="2"/>
+      <c r="D61" s="22">
+        <v>239</v>
+      </c>
       <c r="E61" t="s">
         <v>119</v>
       </c>
@@ -39978,7 +40101,9 @@
         <f>AVERAGE('US Sub-4 Milers'!G546:G564)</f>
         <v>2.7648574561403515E-3</v>
       </c>
-      <c r="D62" s="2"/>
+      <c r="D62" s="22">
+        <v>238.9</v>
+      </c>
       <c r="E62" t="s">
         <v>120</v>
       </c>
@@ -39995,7 +40120,9 @@
         <f>AVERAGE('US Sub-4 Milers'!G565:G600)</f>
         <v>2.7602752057613168E-3</v>
       </c>
-      <c r="D63" s="2"/>
+      <c r="D63" s="22">
+        <v>238.5</v>
+      </c>
       <c r="E63" t="s">
         <v>120</v>
       </c>
@@ -40012,7 +40139,9 @@
         <f>AVERAGE('US Sub-4 Milers'!G601:G660)</f>
         <v>2.7579398148148155E-3</v>
       </c>
-      <c r="D64" s="2"/>
+      <c r="D64" s="22">
+        <v>238.3</v>
+      </c>
       <c r="E64" t="s">
         <v>120</v>
       </c>
@@ -40096,8 +40225,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50CD72C3-FD29-42D6-B204-872167580F24}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -40128,6 +40257,9 @@
         <f>AVERAGE('US Sub-4 Milers'!G2)</f>
         <v>2.7627314814814819E-3</v>
       </c>
+      <c r="D2">
+        <v>238.7</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -40141,6 +40273,9 @@
         <f>AVERAGE('US Sub-4 Milers'!G3:G32)</f>
         <v>2.7626427469135792E-3</v>
       </c>
+      <c r="D3">
+        <v>238.7</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -40154,6 +40289,9 @@
         <f>AVERAGE('US Sub-4 Milers'!G33:G100)</f>
         <v>2.7644488698257085E-3</v>
       </c>
+      <c r="D4">
+        <v>238.8</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -40167,6 +40305,9 @@
         <f>AVERAGE('US Sub-4 Milers'!G101:G169)</f>
         <v>2.7597457058507789E-3</v>
       </c>
+      <c r="D5">
+        <v>238.4</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -40180,6 +40321,9 @@
         <f>AVERAGE('US Sub-4 Milers'!G170:G232)</f>
         <v>2.7619837595532037E-3</v>
       </c>
+      <c r="D6">
+        <v>238.6</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -40193,6 +40337,9 @@
         <f>AVERAGE('US Sub-4 Milers'!G233:G330)</f>
         <v>2.7626263699924414E-3</v>
       </c>
+      <c r="D7">
+        <v>238.7</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -40206,6 +40353,9 @@
         <f>AVERAGE('US Sub-4 Milers'!G331:G545)</f>
         <v>2.7643136304909572E-3</v>
       </c>
+      <c r="D8">
+        <v>238.8</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -40218,6 +40368,9 @@
       <c r="C9" s="2">
         <f>AVERAGE('US Sub-4 Milers'!G546:G660)</f>
         <v>2.7598138083735914E-3</v>
+      </c>
+      <c r="D9">
+        <v>238.4</v>
       </c>
     </row>
   </sheetData>
@@ -40779,8 +40932,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B390BB9-06BB-467C-AFF4-729369118CE1}">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -40832,11 +40985,15 @@
       <c r="B2" s="7">
         <v>2.7638888888888886E-3</v>
       </c>
-      <c r="C2" s="12"/>
+      <c r="C2" s="12">
+        <v>238.8</v>
+      </c>
       <c r="D2" s="7">
         <v>2.7638888888888886E-3</v>
       </c>
-      <c r="E2" s="12"/>
+      <c r="E2" s="12">
+        <v>238.8</v>
+      </c>
       <c r="F2" s="7">
         <f>B2-D2</f>
         <v>0</v>
@@ -40858,11 +41015,15 @@
       <c r="B3" s="7">
         <v>2.7766203703703703E-3</v>
       </c>
-      <c r="C3" s="12"/>
+      <c r="C3" s="12">
+        <v>239.9</v>
+      </c>
       <c r="D3" s="7">
         <v>2.7586805555555559E-3</v>
       </c>
-      <c r="E3" s="12"/>
+      <c r="E3" s="12">
+        <v>238.4</v>
+      </c>
       <c r="F3" s="7">
         <f>B3-D3</f>
         <v>1.7939814814814381E-5</v>
@@ -40884,11 +41045,15 @@
       <c r="B4" s="7">
         <v>2.7685185185185187E-3</v>
       </c>
-      <c r="C4" s="12"/>
+      <c r="C4" s="12">
+        <v>239.2</v>
+      </c>
       <c r="D4" s="7">
         <v>2.7192129629629632E-3</v>
       </c>
-      <c r="E4" s="12"/>
+      <c r="E4" s="12">
+        <v>234.9</v>
+      </c>
       <c r="F4" s="7">
         <f t="shared" ref="F4:F13" si="0">B4-D4</f>
         <v>4.9305555555555474E-5</v>
@@ -40910,11 +41075,15 @@
       <c r="B5" s="7">
         <v>2.753703703703704E-3</v>
       </c>
-      <c r="C5" s="12"/>
+      <c r="C5" s="12">
+        <v>237.9</v>
+      </c>
       <c r="D5" s="7">
         <v>2.6681712962962965E-3</v>
       </c>
-      <c r="E5" s="12"/>
+      <c r="E5" s="12">
+        <v>230.5</v>
+      </c>
       <c r="F5" s="7">
         <f t="shared" si="0"/>
         <v>8.5532407407407432E-5</v>
@@ -40936,11 +41105,15 @@
       <c r="B6" s="7">
         <v>2.7627314814814819E-3</v>
       </c>
-      <c r="C6" s="12"/>
+      <c r="C6" s="12">
+        <v>238.7</v>
+      </c>
       <c r="D6" s="7">
         <v>2.7395833333333335E-3</v>
       </c>
-      <c r="E6" s="12"/>
+      <c r="E6" s="12">
+        <v>236.7</v>
+      </c>
       <c r="F6" s="7">
         <f t="shared" si="0"/>
         <v>2.3148148148148442E-5</v>
@@ -40962,11 +41135,15 @@
       <c r="B7" s="7">
         <v>2.7745370370370372E-3</v>
       </c>
-      <c r="C7" s="12"/>
+      <c r="C7" s="12">
+        <v>239.7</v>
+      </c>
       <c r="D7" s="7">
         <v>2.7745370370370372E-3</v>
       </c>
-      <c r="E7" s="12"/>
+      <c r="E7" s="12">
+        <v>239.7</v>
+      </c>
       <c r="F7" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -40988,11 +41165,15 @@
       <c r="B8" s="7">
         <v>2.7442129629629626E-3</v>
       </c>
-      <c r="C8" s="12"/>
+      <c r="C8" s="12">
+        <v>237.1</v>
+      </c>
       <c r="D8" s="7">
         <v>2.6775462962962964E-3</v>
       </c>
-      <c r="E8" s="12"/>
+      <c r="E8" s="12">
+        <v>231.3</v>
+      </c>
       <c r="F8" s="7">
         <f t="shared" si="0"/>
         <v>6.6666666666666263E-5</v>
@@ -41014,11 +41195,15 @@
       <c r="B9" s="7">
         <v>2.7484953703703703E-3</v>
       </c>
-      <c r="C9" s="12"/>
+      <c r="C9" s="12">
+        <v>237.5</v>
+      </c>
       <c r="D9" s="7">
         <v>2.6608796296296294E-3</v>
       </c>
-      <c r="E9" s="12"/>
+      <c r="E9" s="12">
+        <v>229.9</v>
+      </c>
       <c r="F9" s="7">
         <f t="shared" si="0"/>
         <v>8.761574074074097E-5</v>
@@ -41040,11 +41225,15 @@
       <c r="B10" s="7">
         <v>2.7563657407407411E-3</v>
       </c>
-      <c r="C10" s="12"/>
+      <c r="C10" s="12">
+        <v>238.2</v>
+      </c>
       <c r="D10" s="7">
         <v>2.7212962962962963E-3</v>
       </c>
-      <c r="E10" s="12"/>
+      <c r="E10" s="12">
+        <v>235.1</v>
+      </c>
       <c r="F10" s="7">
         <f t="shared" si="0"/>
         <v>3.5069444444444774E-5</v>
@@ -41066,11 +41255,15 @@
       <c r="B11" s="7">
         <v>2.772337962962963E-3</v>
       </c>
-      <c r="C11" s="12"/>
+      <c r="C11" s="12">
+        <v>239.5</v>
+      </c>
       <c r="D11" s="7">
         <v>2.7506944444444445E-3</v>
       </c>
-      <c r="E11" s="12"/>
+      <c r="E11" s="12">
+        <v>237.7</v>
+      </c>
       <c r="F11" s="7">
         <f t="shared" si="0"/>
         <v>2.1643518518518496E-5</v>
@@ -41092,11 +41285,15 @@
       <c r="B12" s="7">
         <v>2.7280092592592594E-3</v>
       </c>
-      <c r="C12" s="12"/>
+      <c r="C12" s="12">
+        <v>235.7</v>
+      </c>
       <c r="D12" s="7">
         <v>2.7221064814814812E-3</v>
       </c>
-      <c r="E12" s="12"/>
+      <c r="E12" s="12">
+        <v>235.2</v>
+      </c>
       <c r="F12" s="7">
         <f t="shared" si="0"/>
         <v>5.9027777777782842E-6</v>
@@ -41118,11 +41315,15 @@
       <c r="B13" s="7">
         <v>2.7666666666666668E-3</v>
       </c>
-      <c r="C13" s="12"/>
+      <c r="C13" s="12">
+        <v>239</v>
+      </c>
       <c r="D13" s="7">
         <v>2.7391203703703705E-3</v>
       </c>
-      <c r="E13" s="12"/>
+      <c r="E13" s="12">
+        <v>236.7</v>
+      </c>
       <c r="F13" s="7">
         <f t="shared" si="0"/>
         <v>2.7546296296296346E-5</v>
@@ -41147,7 +41348,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -41196,12 +41397,16 @@
         <f>AVERAGE('Fastest American Father Son Duo'!B6:B7)</f>
         <v>2.7686342592592597E-3</v>
       </c>
-      <c r="C2" s="12"/>
+      <c r="C2" s="12">
+        <v>239.2</v>
+      </c>
       <c r="D2" s="7">
         <f>AVERAGE('Fastest American Father Son Duo'!C6:C7)</f>
         <v>2.7570601851851853E-3</v>
       </c>
-      <c r="E2" s="12"/>
+      <c r="E2" s="12">
+        <v>238.2</v>
+      </c>
       <c r="F2" s="7">
         <f>AVERAGE('Fastest American Father Son Duo'!D6:D7)</f>
         <v>1.1574074074074221E-5</v>
@@ -41221,12 +41426,16 @@
         <f>AVERAGE('Fastest American Father Son Duo'!B2:B3)</f>
         <v>2.7702546296296295E-3</v>
       </c>
-      <c r="C3" s="12"/>
+      <c r="C3" s="12">
+        <v>239.3</v>
+      </c>
       <c r="D3" s="7">
         <f>AVERAGE('Fastest American Father Son Duo'!C2:C3)</f>
         <v>2.7612847222222223E-3</v>
       </c>
-      <c r="E3" s="12"/>
+      <c r="E3" s="12">
+        <v>238.6</v>
+      </c>
       <c r="F3" s="7">
         <f>AVERAGE('Fastest American Father Son Duo'!D2:D3)</f>
         <v>8.9699074074071905E-6</v>
@@ -41246,12 +41455,16 @@
         <f>AVERAGE('Fastest American Father Son Duo'!B4:B5)</f>
         <v>2.7611111111111113E-3</v>
       </c>
-      <c r="C4" s="12"/>
+      <c r="C4" s="12">
+        <v>238.6</v>
+      </c>
       <c r="D4" s="7">
         <f>AVERAGE('Fastest American Father Son Duo'!C4:C5)</f>
         <v>2.6936921296296301E-3</v>
       </c>
-      <c r="E4" s="12"/>
+      <c r="E4" s="12">
+        <v>232.7</v>
+      </c>
       <c r="F4" s="7">
         <f>AVERAGE('Fastest American Father Son Duo'!D4:D5)</f>
         <v>6.7418981481481453E-5</v>
@@ -41271,12 +41484,16 @@
         <f>AVERAGE('Fastest American Father Son Duo'!B10:B11)</f>
         <v>2.764351851851852E-3</v>
       </c>
-      <c r="C5" s="12"/>
+      <c r="C5" s="12">
+        <v>238.8</v>
+      </c>
       <c r="D5" s="7">
         <f>AVERAGE('Fastest American Father Son Duo'!C10:C11)</f>
         <v>2.7359953703703704E-3</v>
       </c>
-      <c r="E5" s="12"/>
+      <c r="E5" s="12">
+        <v>236.4</v>
+      </c>
       <c r="F5" s="7">
         <f>AVERAGE('Fastest American Father Son Duo'!D10:D11)</f>
         <v>2.8356481481481635E-5</v>
@@ -41296,12 +41513,16 @@
         <f>AVERAGE('Fastest American Father Son Duo'!B8:B9)</f>
         <v>2.7463541666666665E-3</v>
       </c>
-      <c r="C6" s="12"/>
+      <c r="C6" s="12">
+        <v>237.3</v>
+      </c>
       <c r="D6" s="7">
         <f>AVERAGE('Fastest American Father Son Duo'!C8:C9)</f>
         <v>2.6692129629629626E-3</v>
       </c>
-      <c r="E6" s="12"/>
+      <c r="E6" s="12">
+        <v>230.6</v>
+      </c>
       <c r="F6" s="7">
         <f>AVERAGE('Fastest American Father Son Duo'!D8:D9)</f>
         <v>7.7141203703703616E-5</v>
@@ -41321,12 +41542,16 @@
         <f>AVERAGE('Fastest American Father Son Duo'!B12:B13)</f>
         <v>2.7473379629629631E-3</v>
       </c>
-      <c r="C7" s="12"/>
+      <c r="C7" s="12">
+        <v>237.4</v>
+      </c>
       <c r="D7" s="7">
         <f>AVERAGE('Fastest American Father Son Duo'!C12:C13)</f>
         <v>2.7306134259259258E-3</v>
       </c>
-      <c r="E7" s="12"/>
+      <c r="E7" s="12">
+        <v>235.9</v>
+      </c>
       <c r="F7" s="7">
         <f>AVERAGE('Fastest American Father Son Duo'!D12:D13)</f>
         <v>1.6724537037037315E-5</v>

</xml_diff>

<commit_message>
Major updates to the project all around!
</commit_message>
<xml_diff>
--- a/spreadsheets/US_Sub4_Milers.xlsx
+++ b/spreadsheets/US_Sub4_Milers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ljcoo\NSS\Projects\United_States_Sub_4_Milers_Database\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AECAE3D-6C43-4B00-B9E9-ECEDA712E9BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{109EDF55-D17D-4462-A7BD-0E203CAEA123}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3432" yWindow="1416" windowWidth="17280" windowHeight="10044" firstSheet="2" activeTab="4" xr2:uid="{FC2F9DD0-DB5D-4A46-B58C-40A2751618EA}"/>
+    <workbookView xWindow="3432" yWindow="1416" windowWidth="17280" windowHeight="10044" activeTab="6" xr2:uid="{FC2F9DD0-DB5D-4A46-B58C-40A2751618EA}"/>
   </bookViews>
   <sheets>
     <sheet name="US Sub-4 Milers" sheetId="1" r:id="rId1"/>
@@ -19,9 +19,10 @@
     <sheet name="Faster &amp; Slower than Avg" sheetId="12" r:id="rId4"/>
     <sheet name="Sub-4 By Decade" sheetId="3" r:id="rId5"/>
     <sheet name="Avg # of Runners Sub-4 Per Dec" sheetId="4" r:id="rId6"/>
-    <sheet name="Fastest American Father Son Duo" sheetId="6" r:id="rId7"/>
-    <sheet name="FS Duo General" sheetId="7" r:id="rId8"/>
-    <sheet name="FS Duo Avg" sheetId="10" r:id="rId9"/>
+    <sheet name="Summary Tile Info" sheetId="13" r:id="rId7"/>
+    <sheet name="Fastest American Father Son Duo" sheetId="6" r:id="rId8"/>
+    <sheet name="FS Duo General" sheetId="7" r:id="rId9"/>
+    <sheet name="FS Duo Avg" sheetId="10" r:id="rId10"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'US Sub-4 Milers'!$G$1:$G$660</definedName>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6147" uniqueCount="1743">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6152" uniqueCount="1748">
   <si>
     <t>Stockton</t>
   </si>
@@ -5272,6 +5273,21 @@
   </si>
   <si>
     <t>ADFF_Sec</t>
+  </si>
+  <si>
+    <t>Total Number of Sub-4 Milers</t>
+  </si>
+  <si>
+    <t>Average Mile Time</t>
+  </si>
+  <si>
+    <t>Slowest Time</t>
+  </si>
+  <si>
+    <t>Fastest Time</t>
+  </si>
+  <si>
+    <t>Year of First American Sub-4 Mile</t>
   </si>
 </sst>
 </file>
@@ -5369,7 +5385,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -5398,6 +5414,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -38801,12 +38818,237 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77D85CE0-4DCE-4B0B-810D-7D0F716F7306}">
+  <dimension ref="A1:H7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.21875" customWidth="1"/>
+    <col min="2" max="2" width="26.21875" customWidth="1"/>
+    <col min="3" max="3" width="26.21875" style="22" customWidth="1"/>
+    <col min="4" max="4" width="11.21875" customWidth="1"/>
+    <col min="5" max="5" width="11.21875" style="22" customWidth="1"/>
+    <col min="6" max="6" width="39.6640625" customWidth="1"/>
+    <col min="7" max="7" width="39.6640625" style="22" customWidth="1"/>
+    <col min="8" max="8" width="26" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="18" t="s">
+        <v>1703</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>1727</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>1740</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>1728</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>1741</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>1729</v>
+      </c>
+      <c r="G1" s="19" t="s">
+        <v>1742</v>
+      </c>
+      <c r="H1" s="19" t="s">
+        <v>1730</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="8" t="s">
+        <v>1713</v>
+      </c>
+      <c r="B2" s="7">
+        <f>AVERAGE('Fastest American Father Son Duo'!B6:B7)</f>
+        <v>2.7686342592592597E-3</v>
+      </c>
+      <c r="C2" s="12">
+        <v>239.2</v>
+      </c>
+      <c r="D2" s="7">
+        <f>AVERAGE('Fastest American Father Son Duo'!C6:C7)</f>
+        <v>2.7570601851851853E-3</v>
+      </c>
+      <c r="E2" s="12">
+        <v>238.2</v>
+      </c>
+      <c r="F2" s="7">
+        <f>AVERAGE('Fastest American Father Son Duo'!D6:D7)</f>
+        <v>1.1574074074074221E-5</v>
+      </c>
+      <c r="G2" s="12">
+        <v>1</v>
+      </c>
+      <c r="H2" s="12">
+        <v>15576</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="8" t="s">
+        <v>436</v>
+      </c>
+      <c r="B3" s="7">
+        <f>AVERAGE('Fastest American Father Son Duo'!B2:B3)</f>
+        <v>2.7702546296296295E-3</v>
+      </c>
+      <c r="C3" s="12">
+        <v>239.3</v>
+      </c>
+      <c r="D3" s="7">
+        <f>AVERAGE('Fastest American Father Son Duo'!C2:C3)</f>
+        <v>2.7612847222222223E-3</v>
+      </c>
+      <c r="E3" s="12">
+        <v>238.6</v>
+      </c>
+      <c r="F3" s="7">
+        <f>AVERAGE('Fastest American Father Son Duo'!D2:D3)</f>
+        <v>8.9699074074071905E-6</v>
+      </c>
+      <c r="G3" s="12">
+        <v>0.8</v>
+      </c>
+      <c r="H3" s="12">
+        <v>12746</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="8" t="s">
+        <v>1709</v>
+      </c>
+      <c r="B4" s="7">
+        <f>AVERAGE('Fastest American Father Son Duo'!B4:B5)</f>
+        <v>2.7611111111111113E-3</v>
+      </c>
+      <c r="C4" s="12">
+        <v>238.6</v>
+      </c>
+      <c r="D4" s="7">
+        <f>AVERAGE('Fastest American Father Son Duo'!C4:C5)</f>
+        <v>2.6936921296296301E-3</v>
+      </c>
+      <c r="E4" s="12">
+        <v>232.7</v>
+      </c>
+      <c r="F4" s="7">
+        <f>AVERAGE('Fastest American Father Son Duo'!D4:D5)</f>
+        <v>6.7418981481481453E-5</v>
+      </c>
+      <c r="G4" s="12">
+        <v>5.8</v>
+      </c>
+      <c r="H4" s="12">
+        <v>12320</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="8" t="s">
+        <v>1721</v>
+      </c>
+      <c r="B5" s="7">
+        <f>AVERAGE('Fastest American Father Son Duo'!B10:B11)</f>
+        <v>2.764351851851852E-3</v>
+      </c>
+      <c r="C5" s="12">
+        <v>238.8</v>
+      </c>
+      <c r="D5" s="7">
+        <f>AVERAGE('Fastest American Father Son Duo'!C10:C11)</f>
+        <v>2.7359953703703704E-3</v>
+      </c>
+      <c r="E5" s="12">
+        <v>236.4</v>
+      </c>
+      <c r="F5" s="7">
+        <f>AVERAGE('Fastest American Father Son Duo'!D10:D11)</f>
+        <v>2.8356481481481635E-5</v>
+      </c>
+      <c r="G5" s="12">
+        <v>2.5</v>
+      </c>
+      <c r="H5" s="12">
+        <v>8665</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="8" t="s">
+        <v>1716</v>
+      </c>
+      <c r="B6" s="7">
+        <f>AVERAGE('Fastest American Father Son Duo'!B8:B9)</f>
+        <v>2.7463541666666665E-3</v>
+      </c>
+      <c r="C6" s="12">
+        <v>237.3</v>
+      </c>
+      <c r="D6" s="7">
+        <f>AVERAGE('Fastest American Father Son Duo'!C8:C9)</f>
+        <v>2.6692129629629626E-3</v>
+      </c>
+      <c r="E6" s="12">
+        <v>230.6</v>
+      </c>
+      <c r="F6" s="7">
+        <f>AVERAGE('Fastest American Father Son Duo'!D8:D9)</f>
+        <v>7.7141203703703616E-5</v>
+      </c>
+      <c r="G6" s="12">
+        <v>6.7</v>
+      </c>
+      <c r="H6" s="12">
+        <v>12313</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="8" t="s">
+        <v>1731</v>
+      </c>
+      <c r="B7" s="7">
+        <f>AVERAGE('Fastest American Father Son Duo'!B12:B13)</f>
+        <v>2.7473379629629631E-3</v>
+      </c>
+      <c r="C7" s="12">
+        <v>237.4</v>
+      </c>
+      <c r="D7" s="7">
+        <f>AVERAGE('Fastest American Father Son Duo'!C12:C13)</f>
+        <v>2.7306134259259258E-3</v>
+      </c>
+      <c r="E7" s="12">
+        <v>235.9</v>
+      </c>
+      <c r="F7" s="7">
+        <f>AVERAGE('Fastest American Father Son Duo'!D12:D13)</f>
+        <v>1.6724537037037315E-5</v>
+      </c>
+      <c r="G7" s="12">
+        <v>1.4</v>
+      </c>
+      <c r="H7" s="12">
+        <v>12079</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D8B6DD3-D17E-46BB-8A78-8AF8C223F2B2}">
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -40225,7 +40467,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50CD72C3-FD29-42D6-B204-872167580F24}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -40474,6 +40716,62 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8383042-3FE7-492E-819C-4171300EAE0D}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="11.33203125" style="22" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>1743</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1744</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>1745</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>1746</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>1747</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>659</v>
+      </c>
+      <c r="B2" s="24">
+        <f>AVERAGE('US Sub-4 Milers'!G2:G660)</f>
+        <v>2.7625119428988936E-3</v>
+      </c>
+      <c r="C2" s="2">
+        <f>'General Stats'!$B$5</f>
+        <v>2.7770833333333332E-3</v>
+      </c>
+      <c r="D2" s="2">
+        <f>'General Stats'!$B$4</f>
+        <v>2.6484953703703705E-3</v>
+      </c>
+      <c r="E2" s="22">
+        <v>1957</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88E39F90-A8EC-480A-B778-EE85CEA603AD}">
   <dimension ref="A1:F25"/>
   <sheetViews>
@@ -40928,7 +41226,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B390BB9-06BB-467C-AFF4-729369118CE1}">
   <dimension ref="A1:I13"/>
   <sheetViews>
@@ -41341,229 +41639,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77D85CE0-4DCE-4B0B-810D-7D0F716F7306}">
-  <dimension ref="A1:H7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="10.21875" customWidth="1"/>
-    <col min="2" max="2" width="26.21875" customWidth="1"/>
-    <col min="3" max="3" width="26.21875" style="22" customWidth="1"/>
-    <col min="4" max="4" width="11.21875" customWidth="1"/>
-    <col min="5" max="5" width="11.21875" style="22" customWidth="1"/>
-    <col min="6" max="6" width="39.6640625" customWidth="1"/>
-    <col min="7" max="7" width="39.6640625" style="22" customWidth="1"/>
-    <col min="8" max="8" width="26" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="18" t="s">
-        <v>1703</v>
-      </c>
-      <c r="B1" s="18" t="s">
-        <v>1727</v>
-      </c>
-      <c r="C1" s="19" t="s">
-        <v>1740</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>1728</v>
-      </c>
-      <c r="E1" s="19" t="s">
-        <v>1741</v>
-      </c>
-      <c r="F1" s="18" t="s">
-        <v>1729</v>
-      </c>
-      <c r="G1" s="19" t="s">
-        <v>1742</v>
-      </c>
-      <c r="H1" s="19" t="s">
-        <v>1730</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="8" t="s">
-        <v>1713</v>
-      </c>
-      <c r="B2" s="7">
-        <f>AVERAGE('Fastest American Father Son Duo'!B6:B7)</f>
-        <v>2.7686342592592597E-3</v>
-      </c>
-      <c r="C2" s="12">
-        <v>239.2</v>
-      </c>
-      <c r="D2" s="7">
-        <f>AVERAGE('Fastest American Father Son Duo'!C6:C7)</f>
-        <v>2.7570601851851853E-3</v>
-      </c>
-      <c r="E2" s="12">
-        <v>238.2</v>
-      </c>
-      <c r="F2" s="7">
-        <f>AVERAGE('Fastest American Father Son Duo'!D6:D7)</f>
-        <v>1.1574074074074221E-5</v>
-      </c>
-      <c r="G2" s="12">
-        <v>1</v>
-      </c>
-      <c r="H2" s="12">
-        <v>15576</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="8" t="s">
-        <v>436</v>
-      </c>
-      <c r="B3" s="7">
-        <f>AVERAGE('Fastest American Father Son Duo'!B2:B3)</f>
-        <v>2.7702546296296295E-3</v>
-      </c>
-      <c r="C3" s="12">
-        <v>239.3</v>
-      </c>
-      <c r="D3" s="7">
-        <f>AVERAGE('Fastest American Father Son Duo'!C2:C3)</f>
-        <v>2.7612847222222223E-3</v>
-      </c>
-      <c r="E3" s="12">
-        <v>238.6</v>
-      </c>
-      <c r="F3" s="7">
-        <f>AVERAGE('Fastest American Father Son Duo'!D2:D3)</f>
-        <v>8.9699074074071905E-6</v>
-      </c>
-      <c r="G3" s="12">
-        <v>0.8</v>
-      </c>
-      <c r="H3" s="12">
-        <v>12746</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="8" t="s">
-        <v>1709</v>
-      </c>
-      <c r="B4" s="7">
-        <f>AVERAGE('Fastest American Father Son Duo'!B4:B5)</f>
-        <v>2.7611111111111113E-3</v>
-      </c>
-      <c r="C4" s="12">
-        <v>238.6</v>
-      </c>
-      <c r="D4" s="7">
-        <f>AVERAGE('Fastest American Father Son Duo'!C4:C5)</f>
-        <v>2.6936921296296301E-3</v>
-      </c>
-      <c r="E4" s="12">
-        <v>232.7</v>
-      </c>
-      <c r="F4" s="7">
-        <f>AVERAGE('Fastest American Father Son Duo'!D4:D5)</f>
-        <v>6.7418981481481453E-5</v>
-      </c>
-      <c r="G4" s="12">
-        <v>5.8</v>
-      </c>
-      <c r="H4" s="12">
-        <v>12320</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="8" t="s">
-        <v>1721</v>
-      </c>
-      <c r="B5" s="7">
-        <f>AVERAGE('Fastest American Father Son Duo'!B10:B11)</f>
-        <v>2.764351851851852E-3</v>
-      </c>
-      <c r="C5" s="12">
-        <v>238.8</v>
-      </c>
-      <c r="D5" s="7">
-        <f>AVERAGE('Fastest American Father Son Duo'!C10:C11)</f>
-        <v>2.7359953703703704E-3</v>
-      </c>
-      <c r="E5" s="12">
-        <v>236.4</v>
-      </c>
-      <c r="F5" s="7">
-        <f>AVERAGE('Fastest American Father Son Duo'!D10:D11)</f>
-        <v>2.8356481481481635E-5</v>
-      </c>
-      <c r="G5" s="12">
-        <v>2.5</v>
-      </c>
-      <c r="H5" s="12">
-        <v>8665</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="8" t="s">
-        <v>1716</v>
-      </c>
-      <c r="B6" s="7">
-        <f>AVERAGE('Fastest American Father Son Duo'!B8:B9)</f>
-        <v>2.7463541666666665E-3</v>
-      </c>
-      <c r="C6" s="12">
-        <v>237.3</v>
-      </c>
-      <c r="D6" s="7">
-        <f>AVERAGE('Fastest American Father Son Duo'!C8:C9)</f>
-        <v>2.6692129629629626E-3</v>
-      </c>
-      <c r="E6" s="12">
-        <v>230.6</v>
-      </c>
-      <c r="F6" s="7">
-        <f>AVERAGE('Fastest American Father Son Duo'!D8:D9)</f>
-        <v>7.7141203703703616E-5</v>
-      </c>
-      <c r="G6" s="12">
-        <v>6.7</v>
-      </c>
-      <c r="H6" s="12">
-        <v>12313</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="8" t="s">
-        <v>1731</v>
-      </c>
-      <c r="B7" s="7">
-        <f>AVERAGE('Fastest American Father Son Duo'!B12:B13)</f>
-        <v>2.7473379629629631E-3</v>
-      </c>
-      <c r="C7" s="12">
-        <v>237.4</v>
-      </c>
-      <c r="D7" s="7">
-        <f>AVERAGE('Fastest American Father Son Duo'!C12:C13)</f>
-        <v>2.7306134259259258E-3</v>
-      </c>
-      <c r="E7" s="12">
-        <v>235.9</v>
-      </c>
-      <c r="F7" s="7">
-        <f>AVERAGE('Fastest American Father Son Duo'!D12:D13)</f>
-        <v>1.6724537037037315E-5</v>
-      </c>
-      <c r="G7" s="12">
-        <v>1.4</v>
-      </c>
-      <c r="H7" s="12">
-        <v>12079</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>